<commit_message>
Update Regresi API Testing 16/07
</commit_message>
<xml_diff>
--- a/Data Test/signup.xlsx
+++ b/Data Test/signup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. UNNES\6. Semester 6\2 - MSIB\CAPSTONE PROJECT\testing-lms\Data Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169F0248-60B9-49EB-B0F0-C66DBAF87EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E064AA7B-49B2-405C-91D5-83035487FA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1890" yWindow="1245" windowWidth="18000" windowHeight="9270" xr2:uid="{45076FA3-564A-4E50-94CC-5AE5A21FCC3F}"/>
   </bookViews>
@@ -131,7 +131,7 @@
     <t>Joong123!</t>
   </si>
   <si>
-    <t>joong3@gmail.com</t>
+    <t>joong7@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>